<commit_message>
Correction in Excel file
</commit_message>
<xml_diff>
--- a/ClassesTaken/edX/2014/LearnFromData/hw03/hw03.xlsx
+++ b/ClassesTaken/edX/2014/LearnFromData/hw03/hw03.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Workspace\Solutions\ClassesTaken\edX\2014\LearnFromData\hw03\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\Solutions\ClassesTaken\edX\2014\LearnFromData\hw03\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -380,16 +380,16 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.36328125" customWidth="1"/>
-    <col min="2" max="2" width="11.36328125" customWidth="1"/>
+    <col min="1" max="1" width="9.3828125" customWidth="1"/>
+    <col min="2" max="2" width="11.3828125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -409,7 +409,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0.05</v>
       </c>
@@ -424,14 +424,14 @@
         <v>839.94101557598526</v>
       </c>
       <c r="E2">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="F2">
         <f>2*$C2*EXP(-2*$A2*$A2*$E2)</f>
-        <v>3.0141484924178168E-2</v>
+        <v>2.9991153640955382E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>0.05</v>
       </c>
@@ -446,14 +446,14 @@
         <v>1300.4580341747944</v>
       </c>
       <c r="E3">
-        <v>839</v>
+        <v>1300</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F4" si="1">2*$C3*EXP(-2*$A3*$A3*$E3)</f>
-        <v>0.30141484924178169</v>
+        <v>3.0068783859551421E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>0.05</v>
       </c>
@@ -468,11 +468,11 @@
         <v>1760.9750527736037</v>
       </c>
       <c r="E4">
-        <v>839</v>
+        <v>1761</v>
       </c>
       <c r="F4">
         <f t="shared" si="1"/>
-        <v>3.0141484924178168</v>
+        <v>2.9996258149417341E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>